<commit_message>
Rename - Gold, Soul
</commit_message>
<xml_diff>
--- a/ExcelToCSV/SrcFolder/테이블_0323_v22.xlsx
+++ b/ExcelToCSV/SrcFolder/테이블_0323_v22.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejup\Desktop\GameJam\ExcelToCSV\SrcFolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevD\TowerDefense\ExcelToCSV\SrcFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908661CC-4B77-4826-AF19-3CA08901195C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4"/>
+    <workbookView xWindow="32655" yWindow="3090" windowWidth="21870" windowHeight="12150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConfigTable" sheetId="18" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <sheet name="GachaList" sheetId="28" r:id="rId9"/>
     <sheet name="reference" sheetId="31" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ejup</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -95,12 +96,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ejup</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -141,12 +142,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ejup</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -930,10 +931,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>dropGoldCnt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>rewardId</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1447,11 +1444,15 @@
   <si>
     <t>Indian_Egg_2</t>
   </si>
+  <si>
+    <t>dropSoulCnt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -2137,18 +2138,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2193,7 +2194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.399999999999999">
+    <row r="4" spans="1:4" ht="16.5">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999">
+    <row r="5" spans="1:4" ht="16.5">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999">
+    <row r="6" spans="1:4" ht="16.5">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2235,9 +2236,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999">
+    <row r="7" spans="1:4" ht="16.5">
       <c r="A7" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -2246,7 +2247,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2257,44 +2258,44 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="45"/>
-    <col min="2" max="2" width="16.88671875" style="45" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="45" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="45"/>
+    <col min="1" max="1" width="8.85546875" style="45"/>
+    <col min="2" max="2" width="16.85546875" style="45" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="45" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="45"/>
     <col min="5" max="7" width="12" style="45" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="45"/>
+    <col min="8" max="16384" width="8.85546875" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.8" thickBot="1">
+    <row r="1" spans="1:7" ht="12.75" thickBot="1">
       <c r="A1" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="C1" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>178</v>
-      </c>
       <c r="E1" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="45" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="13.8" thickBot="1">
+    </row>
+    <row r="2" spans="1:7" ht="12.75" thickBot="1">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F2" s="45">
         <v>3</v>
@@ -2314,7 +2315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.8" thickBot="1">
+    <row r="3" spans="1:7" ht="12.75" thickBot="1">
       <c r="A3" s="46">
         <v>2</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F3" s="45">
         <v>100</v>
@@ -2334,7 +2335,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.8" thickBot="1">
+    <row r="4" spans="1:7" ht="12.75" thickBot="1">
       <c r="A4" s="46">
         <v>3</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="45">
         <v>0.2</v>
@@ -2354,7 +2355,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.8" thickBot="1">
+    <row r="5" spans="1:7" ht="12.75" thickBot="1">
       <c r="A5" s="46">
         <v>4</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>55</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" s="45">
         <v>1</v>
@@ -2376,7 +2377,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="E6" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F6" s="45">
         <v>25</v>
@@ -2387,7 +2388,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="E7" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7" s="45">
         <v>5</v>
@@ -2398,7 +2399,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="E8" s="45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8" s="45">
         <v>0.2</v>
@@ -2409,7 +2410,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="E9" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9" s="45">
         <v>1</v>
@@ -2420,7 +2421,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="E10" s="45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10" s="45">
         <v>0.2</v>
@@ -2431,7 +2432,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="E11" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11" s="45">
         <v>1</v>
@@ -2443,19 +2444,19 @@
     <row r="19" spans="1:6">
       <c r="A19" s="48"/>
       <c r="B19" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="48" t="s">
-        <v>182</v>
-      </c>
       <c r="E19" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="48" t="s">
         <v>195</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2738,19 +2739,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2857,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2899,7 +2900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15">
+    <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
         <v>28</v>
       </c>
@@ -2941,7 +2942,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
@@ -2960,16 +2961,16 @@
         <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="49" t="s">
         <v>212</v>
       </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="49" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -2983,62 +2984,62 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.399999999999999">
+    <row r="15" spans="1:7" ht="16.5">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17.399999999999999">
+    </row>
+    <row r="16" spans="1:7" ht="16.5">
       <c r="A16" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5">
+      <c r="A17" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="17.399999999999999">
-      <c r="A17" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5">
+      <c r="A18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" ht="17.399999999999999">
-      <c r="A18" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="26"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5">
+      <c r="A19" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="C18" s="4">
-        <v>2</v>
-      </c>
-      <c r="D18" s="26"/>
-    </row>
-    <row r="19" spans="1:4" ht="17.399999999999999">
-      <c r="A19" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="C19" s="4">
         <v>3</v>
@@ -3083,7 +3084,7 @@
       </c>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999">
+    <row r="23" spans="1:4" ht="16.5">
       <c r="A23" s="2" t="s">
         <v>103</v>
       </c>
@@ -3095,7 +3096,7 @@
       </c>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999">
+    <row r="24" spans="1:4" ht="16.5">
       <c r="A24" s="2" t="s">
         <v>103</v>
       </c>
@@ -3131,7 +3132,7 @@
       </c>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999">
+    <row r="27" spans="1:4" ht="16.5">
       <c r="A27" s="2" t="s">
         <v>103</v>
       </c>
@@ -3143,7 +3144,7 @@
       </c>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" ht="17.399999999999999">
+    <row r="28" spans="1:4" ht="16.5">
       <c r="A28" s="2" t="s">
         <v>103</v>
       </c>
@@ -3163,7 +3164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -3173,22 +3174,22 @@
       <selection activeCell="F57" sqref="A57:F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12" style="38" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="38" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="38" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="38" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="38" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" style="38" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" style="38" customWidth="1"/>
-    <col min="12" max="12" width="59.5546875" style="38" customWidth="1"/>
-    <col min="13" max="13" width="50.44140625" style="38" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="38"/>
+    <col min="2" max="2" width="24.5703125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="38" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="38" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="38" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="38" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="38" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" style="38" customWidth="1"/>
+    <col min="12" max="12" width="59.5703125" style="38" customWidth="1"/>
+    <col min="13" max="13" width="50.42578125" style="38" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="35" customFormat="1">
@@ -3196,10 +3197,10 @@
         <v>42</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>55</v>
@@ -3229,7 +3230,7 @@
         <v>47</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3237,10 +3238,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>55</v>
@@ -3258,7 +3259,7 @@
         <v>70</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="37" t="s">
         <v>81</v>
@@ -3278,10 +3279,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="39" t="s">
         <v>2</v>
@@ -3319,7 +3320,7 @@
         <v>1001</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="41" t="str">
         <f>IF(D4=1,"(원거리)","(근거리)")&amp;B4</f>
@@ -3356,7 +3357,7 @@
         <v>Unit/Enemy/Chapter_1/1001_Indian_Archer.prefab</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3364,7 +3365,7 @@
         <v>1002</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="41" t="str">
         <f t="shared" ref="C5:C61" si="0">IF(D5=1,"(원거리)","(근거리)")&amp;B5</f>
@@ -3401,7 +3402,7 @@
         <v>Unit/Enemy/Chapter_1/1002_Indian_Shield.prefab</v>
       </c>
       <c r="M5" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3409,7 +3410,7 @@
         <v>1003</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3446,7 +3447,7 @@
         <v>Unit/Enemy/Chapter_1/1003_Indian_Spear.prefab</v>
       </c>
       <c r="M6" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3454,7 +3455,7 @@
         <v>1004</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3491,7 +3492,7 @@
         <v>Unit/Enemy/Chapter_1/1004_Indian_Sword.prefab</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3499,7 +3500,7 @@
         <v>1005</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3536,7 +3537,7 @@
         <v>Unit/Enemy/Chapter_1/1005_Indian_Mask.prefab</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -3544,7 +3545,7 @@
         <v>1006</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3581,7 +3582,7 @@
         <v>Unit/Enemy/Chapter_1/1006_Indian_Bear.prefab</v>
       </c>
       <c r="M9" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3589,7 +3590,7 @@
         <v>1007</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3626,7 +3627,7 @@
         <v>Unit/Enemy/Chapter_1/1007_Bear.prefab</v>
       </c>
       <c r="M10" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -3634,7 +3635,7 @@
         <v>1008</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3671,7 +3672,7 @@
         <v>Unit/Enemy/Chapter_1/1008_Indian_Master.prefab</v>
       </c>
       <c r="M11" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3679,7 +3680,7 @@
         <v>1009</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3716,7 +3717,7 @@
         <v>Unit/Enemy/Chapter_1/1009_Corgi.prefab</v>
       </c>
       <c r="M12" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -3724,7 +3725,7 @@
         <v>1010</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3761,7 +3762,7 @@
         <v>Unit/Enemy/Chapter_1/1010_Indian_Horse_Sword.prefab</v>
       </c>
       <c r="M13" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -3769,7 +3770,7 @@
         <v>1011</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3806,7 +3807,7 @@
         <v>Unit/Enemy/Chapter_1/1011_Indian_Horse_Spear.prefab</v>
       </c>
       <c r="M14" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -3814,7 +3815,7 @@
         <v>1012</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3851,7 +3852,7 @@
         <v>Unit/Enemy/Chapter_1/1012_Indian_Horse_Archer.prefab</v>
       </c>
       <c r="M15" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -3859,7 +3860,7 @@
         <v>1013</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3896,7 +3897,7 @@
         <v>Unit/Enemy/Chapter_1/1013_Chicken_Black.prefab</v>
       </c>
       <c r="M16" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -3904,7 +3905,7 @@
         <v>1014</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3941,7 +3942,7 @@
         <v>Unit/Enemy/Chapter_1/1014_Chicken_White.prefab</v>
       </c>
       <c r="M17" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -3949,7 +3950,7 @@
         <v>1015</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="41" t="str">
         <f t="shared" si="0"/>
@@ -3986,7 +3987,7 @@
         <v>Unit/Enemy/Chapter_1/1015_Indian_Elephant.prefab</v>
       </c>
       <c r="M18" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -3994,7 +3995,7 @@
         <v>1016</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C19" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4031,7 +4032,7 @@
         <v>Unit/Enemy/Chapter_1/1016_Indian_Egg.prefab</v>
       </c>
       <c r="M19" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -4039,7 +4040,7 @@
         <v>1051</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C20" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4076,7 +4077,7 @@
         <v>Unit/Enemy/Chapter_1/1051_Indian_Archer_2.prefab</v>
       </c>
       <c r="M20" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -4084,7 +4085,7 @@
         <v>1052</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C21" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4121,7 +4122,7 @@
         <v>Unit/Enemy/Chapter_1/1052_Indian_Shield_2.prefab</v>
       </c>
       <c r="M21" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -4129,7 +4130,7 @@
         <v>1053</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C22" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4166,7 +4167,7 @@
         <v>Unit/Enemy/Chapter_1/1053_Indian_Spear_2.prefab</v>
       </c>
       <c r="M22" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -4174,7 +4175,7 @@
         <v>1054</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C23" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4211,7 +4212,7 @@
         <v>Unit/Enemy/Chapter_1/1054_Indian_Sword_2.prefab</v>
       </c>
       <c r="M23" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -4219,7 +4220,7 @@
         <v>1055</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C24" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4256,7 +4257,7 @@
         <v>Unit/Enemy/Chapter_1/1055_Indian_Mask_2.prefab</v>
       </c>
       <c r="M24" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -4264,7 +4265,7 @@
         <v>1056</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C25" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4301,7 +4302,7 @@
         <v>Unit/Enemy/Chapter_1/1056_Indian_Bear_2.prefab</v>
       </c>
       <c r="M25" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -4309,7 +4310,7 @@
         <v>1057</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C26" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4346,7 +4347,7 @@
         <v>Unit/Enemy/Chapter_1/1057_Bear_2.prefab</v>
       </c>
       <c r="M26" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -4354,7 +4355,7 @@
         <v>1058</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C27" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4391,7 +4392,7 @@
         <v>Unit/Enemy/Chapter_1/1058_Indian_Master_2.prefab</v>
       </c>
       <c r="M27" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -4399,7 +4400,7 @@
         <v>1059</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C28" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4436,7 +4437,7 @@
         <v>Unit/Enemy/Chapter_1/1059_Corgi_2.prefab</v>
       </c>
       <c r="M28" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -4444,7 +4445,7 @@
         <v>1060</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C29" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4481,7 +4482,7 @@
         <v>Unit/Enemy/Chapter_1/1060_Indian_Horse_Sword_2.prefab</v>
       </c>
       <c r="M29" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -4489,7 +4490,7 @@
         <v>1061</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C30" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4526,7 +4527,7 @@
         <v>Unit/Enemy/Chapter_1/1061_Indian_Horse_Spear_2.prefab</v>
       </c>
       <c r="M30" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -4534,7 +4535,7 @@
         <v>1062</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C31" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4571,7 +4572,7 @@
         <v>Unit/Enemy/Chapter_1/1062_Indian_Horse_Archer_2.prefab</v>
       </c>
       <c r="M31" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -4579,7 +4580,7 @@
         <v>1063</v>
       </c>
       <c r="B32" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C32" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4616,7 +4617,7 @@
         <v>Unit/Enemy/Chapter_1/1063_Chicken_Black_2.prefab</v>
       </c>
       <c r="M32" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -4624,7 +4625,7 @@
         <v>1064</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C33" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4661,7 +4662,7 @@
         <v>Unit/Enemy/Chapter_1/1064_Chicken_White_2.prefab</v>
       </c>
       <c r="M33" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -4669,7 +4670,7 @@
         <v>1065</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C34" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4706,7 +4707,7 @@
         <v>Unit/Enemy/Chapter_1/1065_Indian_Elephant_2.prefab</v>
       </c>
       <c r="M34" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -4714,7 +4715,7 @@
         <v>1066</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C35" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4751,7 +4752,7 @@
         <v>Unit/Enemy/Chapter_1/1066_Indian_Egg_2.prefab</v>
       </c>
       <c r="M35" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -4759,7 +4760,7 @@
         <v>2001</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4796,7 +4797,7 @@
         <v>Unit/Hero/2001_Slime.prefab</v>
       </c>
       <c r="M36" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -4804,7 +4805,7 @@
         <v>2002</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4841,7 +4842,7 @@
         <v>Unit/Hero/2002_Slime_Archer.prefab</v>
       </c>
       <c r="M37" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -4849,7 +4850,7 @@
         <v>2003</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4886,7 +4887,7 @@
         <v>Unit/Hero/2003_Skeleton_Sword.prefab</v>
       </c>
       <c r="M38" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -4894,7 +4895,7 @@
         <v>2004</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4931,7 +4932,7 @@
         <v>Unit/Hero/2004_Skeleton_Archer.prefab</v>
       </c>
       <c r="M39" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -4939,7 +4940,7 @@
         <v>2005</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="41" t="str">
         <f t="shared" si="0"/>
@@ -4976,7 +4977,7 @@
         <v>Unit/Hero/2005_Skeleton_Witch.prefab</v>
       </c>
       <c r="M40" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -4984,7 +4985,7 @@
         <v>2006</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5021,7 +5022,7 @@
         <v>Unit/Hero/2006_Zombie_Hand.prefab</v>
       </c>
       <c r="M41" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -5029,7 +5030,7 @@
         <v>2007</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5066,7 +5067,7 @@
         <v>Unit/Hero/2007_Zombie_Shield.prefab</v>
       </c>
       <c r="M42" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -5074,7 +5075,7 @@
         <v>2008</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5111,7 +5112,7 @@
         <v>Unit/Hero/2008_Zombie_Sword.prefab</v>
       </c>
       <c r="M43" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -5119,7 +5120,7 @@
         <v>2009</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5156,7 +5157,7 @@
         <v>Unit/Hero/2009_Witch_Fire.prefab</v>
       </c>
       <c r="M44" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -5164,7 +5165,7 @@
         <v>2010</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C45" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5201,7 +5202,7 @@
         <v>Unit/Hero/2010_Witch_Thunder.prefab</v>
       </c>
       <c r="M45" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -5209,7 +5210,7 @@
         <v>2011</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C46" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5246,7 +5247,7 @@
         <v>Unit/Hero/2011_Witch_Poison.prefab</v>
       </c>
       <c r="M46" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -5254,7 +5255,7 @@
         <v>2012</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C47" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5291,7 +5292,7 @@
         <v>Unit/Hero/2012_Goblin_Stone.prefab</v>
       </c>
       <c r="M47" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -5299,7 +5300,7 @@
         <v>2013</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C48" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5336,7 +5337,7 @@
         <v>Unit/Hero/2013_Goblin_Club.prefab</v>
       </c>
       <c r="M48" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -5344,7 +5345,7 @@
         <v>2014</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C49" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5381,7 +5382,7 @@
         <v>Unit/Hero/2014_Goblin_Baby.prefab</v>
       </c>
       <c r="M49" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -5389,7 +5390,7 @@
         <v>2015</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C50" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5426,7 +5427,7 @@
         <v>Unit/Hero/2015_Orc_Stone.prefab</v>
       </c>
       <c r="M50" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -5434,7 +5435,7 @@
         <v>2016</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C51" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5471,7 +5472,7 @@
         <v>Unit/Hero/2016_Orc_Club.prefab</v>
       </c>
       <c r="M51" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -5479,7 +5480,7 @@
         <v>2017</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C52" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5516,7 +5517,7 @@
         <v>Unit/Hero/2017_Dragon.prefab</v>
       </c>
       <c r="M52" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -5524,7 +5525,7 @@
         <v>2018</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C53" s="38" t="str">
         <f t="shared" si="0"/>
@@ -5561,7 +5562,7 @@
         <v>Unit/Hero/2018_Dragon_Fire.prefab</v>
       </c>
       <c r="M53" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -5569,7 +5570,7 @@
         <v>11001</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C54" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5606,7 +5607,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11001_Indian_Wagon.prefab</v>
       </c>
       <c r="M54" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -5614,7 +5615,7 @@
         <v>11002</v>
       </c>
       <c r="B55" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C55" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5651,7 +5652,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11002_Indian_Catapult.prefab</v>
       </c>
       <c r="M55" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -5659,7 +5660,7 @@
         <v>11003</v>
       </c>
       <c r="B56" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C56" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5696,7 +5697,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11003_Indian_Wall.prefab</v>
       </c>
       <c r="M56" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -5704,7 +5705,7 @@
         <v>11004</v>
       </c>
       <c r="B57" s="41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C57" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5741,7 +5742,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11004_Indian_Watchtower.prefab</v>
       </c>
       <c r="M57" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -5749,7 +5750,7 @@
         <v>11005</v>
       </c>
       <c r="B58" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C58" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5786,7 +5787,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11005_Indian_Chicken_House.prefab</v>
       </c>
       <c r="M58" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -5794,7 +5795,7 @@
         <v>11006</v>
       </c>
       <c r="B59" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C59" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5831,7 +5832,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11006_Indian_Jar_1.prefab</v>
       </c>
       <c r="M59" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -5839,7 +5840,7 @@
         <v>11007</v>
       </c>
       <c r="B60" s="41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C60" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5876,7 +5877,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11007_Indian_Jar_2.prefab</v>
       </c>
       <c r="M60" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -5884,7 +5885,7 @@
         <v>11008</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C61" s="41" t="str">
         <f t="shared" si="0"/>
@@ -5921,7 +5922,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11008_Indian_Straw.prefab</v>
       </c>
       <c r="M61" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -5929,7 +5930,7 @@
         <v>11009</v>
       </c>
       <c r="B62" s="38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C62" s="41" t="str">
         <f t="shared" ref="C62" si="12">IF(D62=1,"(원거리)","(근거리)")&amp;B62</f>
@@ -5966,7 +5967,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11009_Indian_Flag_Alter.prefab</v>
       </c>
       <c r="M62" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -5974,7 +5975,7 @@
         <v>11010</v>
       </c>
       <c r="B63" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C63" s="41" t="str">
         <f t="shared" ref="C63:C64" si="16">IF(D63=1,"(원거리)","(근거리)")&amp;B63</f>
@@ -6011,7 +6012,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11010_Indian_House.prefab</v>
       </c>
       <c r="M63" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -6019,7 +6020,7 @@
         <v>11011</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C64" s="41" t="str">
         <f t="shared" si="16"/>
@@ -6056,7 +6057,7 @@
         <v>Unit/Enemy/Chapter_1_Object/11011_Indian_Fire.prefab</v>
       </c>
       <c r="M64" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -6066,37 +6067,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="10" width="15.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" customWidth="1"/>
-    <col min="13" max="14" width="18.6640625" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.5546875" customWidth="1"/>
-    <col min="18" max="19" width="12.33203125" customWidth="1"/>
-    <col min="20" max="20" width="27.5546875" style="20" customWidth="1"/>
-    <col min="21" max="22" width="16.33203125" customWidth="1"/>
-    <col min="23" max="23" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" customWidth="1"/>
+    <col min="18" max="19" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="27.5703125" style="20" customWidth="1"/>
+    <col min="21" max="22" width="16.28515625" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="13" customFormat="1">
@@ -6107,7 +6108,7 @@
         <v>50</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>51</v>
@@ -6119,13 +6120,13 @@
         <v>52</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H1" s="31" t="s">
         <v>53</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J1" s="31" t="s">
         <v>54</v>
@@ -6134,7 +6135,7 @@
         <v>58</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M1" s="31" t="s">
         <v>56</v>
@@ -6149,7 +6150,7 @@
         <v>59</v>
       </c>
       <c r="Q1" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R1" s="14" t="s">
         <v>85</v>
@@ -6167,7 +6168,7 @@
         <v>116</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>118</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -6178,7 +6179,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>1</v>
@@ -6249,7 +6250,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>2</v>
@@ -6365,7 +6366,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R4" s="5">
         <v>0</v>
@@ -6374,7 +6375,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U4" s="5">
         <v>2</v>
@@ -6440,7 +6441,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R5" s="5">
         <v>0</v>
@@ -6449,7 +6450,7 @@
         <v>1</v>
       </c>
       <c r="T5" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U5" s="5">
         <v>2</v>
@@ -6515,7 +6516,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R6" s="5">
         <v>0</v>
@@ -6524,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U6" s="5">
         <v>2</v>
@@ -6590,7 +6591,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R7" s="5">
         <v>0</v>
@@ -6599,7 +6600,7 @@
         <v>1</v>
       </c>
       <c r="T7" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U7" s="5">
         <v>2</v>
@@ -6665,7 +6666,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R8" s="5">
         <v>0</v>
@@ -6674,7 +6675,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U8" s="5">
         <v>2</v>
@@ -6740,7 +6741,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R9" s="5">
         <v>0</v>
@@ -6749,7 +6750,7 @@
         <v>1</v>
       </c>
       <c r="T9" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U9" s="5">
         <v>2</v>
@@ -6815,7 +6816,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R10" s="5">
         <v>0</v>
@@ -6824,7 +6825,7 @@
         <v>1</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U10" s="5">
         <v>2</v>
@@ -6890,7 +6891,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R11" s="5">
         <v>0</v>
@@ -6899,7 +6900,7 @@
         <v>1</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U11" s="5">
         <v>2</v>
@@ -6965,7 +6966,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
@@ -6974,7 +6975,7 @@
         <v>1</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U12" s="5">
         <v>2</v>
@@ -7040,7 +7041,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R13" s="5">
         <v>0</v>
@@ -7049,7 +7050,7 @@
         <v>1</v>
       </c>
       <c r="T13" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U13" s="5">
         <v>2</v>
@@ -7115,7 +7116,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R14" s="5">
         <v>0</v>
@@ -7124,7 +7125,7 @@
         <v>1</v>
       </c>
       <c r="T14" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U14" s="5">
         <v>2</v>
@@ -7190,7 +7191,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R15" s="5">
         <v>0</v>
@@ -7199,7 +7200,7 @@
         <v>1</v>
       </c>
       <c r="T15" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U15" s="5">
         <v>2</v>
@@ -7265,7 +7266,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R16" s="5">
         <v>0</v>
@@ -7274,7 +7275,7 @@
         <v>1</v>
       </c>
       <c r="T16" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U16" s="5">
         <v>2</v>
@@ -7340,7 +7341,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R17" s="5">
         <v>0</v>
@@ -7349,7 +7350,7 @@
         <v>1</v>
       </c>
       <c r="T17" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U17" s="5">
         <v>2</v>
@@ -7415,7 +7416,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R18" s="5">
         <v>0</v>
@@ -7424,7 +7425,7 @@
         <v>1</v>
       </c>
       <c r="T18" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U18" s="5">
         <v>2</v>
@@ -7490,7 +7491,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R19" s="5">
         <v>0</v>
@@ -7499,7 +7500,7 @@
         <v>1</v>
       </c>
       <c r="T19" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U19" s="5">
         <v>2</v>
@@ -7565,7 +7566,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R20" s="5">
         <v>0</v>
@@ -7574,7 +7575,7 @@
         <v>1</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U20" s="5">
         <v>2</v>
@@ -7640,7 +7641,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R21" s="5">
         <v>0</v>
@@ -7649,7 +7650,7 @@
         <v>1</v>
       </c>
       <c r="T21" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U21" s="5">
         <v>2</v>
@@ -7715,7 +7716,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R22" s="5">
         <v>0</v>
@@ -7724,7 +7725,7 @@
         <v>1</v>
       </c>
       <c r="T22" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U22" s="5">
         <v>2</v>
@@ -7790,7 +7791,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R23" s="5">
         <v>0</v>
@@ -7799,7 +7800,7 @@
         <v>1</v>
       </c>
       <c r="T23" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U23" s="5">
         <v>2</v>
@@ -7865,7 +7866,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R24" s="5">
         <v>0</v>
@@ -7874,7 +7875,7 @@
         <v>1</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U24" s="5">
         <v>2</v>
@@ -7940,7 +7941,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R25" s="5">
         <v>0</v>
@@ -7949,7 +7950,7 @@
         <v>1</v>
       </c>
       <c r="T25" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U25" s="5">
         <v>2</v>
@@ -8015,7 +8016,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R26" s="5">
         <v>0</v>
@@ -8024,7 +8025,7 @@
         <v>1</v>
       </c>
       <c r="T26" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U26" s="5">
         <v>2</v>
@@ -8090,7 +8091,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R27" s="5">
         <v>0</v>
@@ -8099,7 +8100,7 @@
         <v>1</v>
       </c>
       <c r="T27" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U27" s="5">
         <v>2</v>
@@ -8165,7 +8166,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R28" s="5">
         <v>0</v>
@@ -8174,7 +8175,7 @@
         <v>1</v>
       </c>
       <c r="T28" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U28" s="5">
         <v>2</v>
@@ -8240,7 +8241,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R29" s="5">
         <v>0</v>
@@ -8249,7 +8250,7 @@
         <v>1</v>
       </c>
       <c r="T29" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U29" s="5">
         <v>2</v>
@@ -8315,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R30" s="5">
         <v>0</v>
@@ -8324,7 +8325,7 @@
         <v>1</v>
       </c>
       <c r="T30" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U30" s="5">
         <v>2</v>
@@ -8390,7 +8391,7 @@
         <v>0</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R31" s="5">
         <v>0</v>
@@ -8399,7 +8400,7 @@
         <v>1</v>
       </c>
       <c r="T31" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U31" s="5">
         <v>2</v>
@@ -8465,7 +8466,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R32" s="5">
         <v>0</v>
@@ -8474,7 +8475,7 @@
         <v>1</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U32" s="5">
         <v>2</v>
@@ -8540,7 +8541,7 @@
         <v>0</v>
       </c>
       <c r="Q33" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R33" s="5">
         <v>0</v>
@@ -8549,7 +8550,7 @@
         <v>1</v>
       </c>
       <c r="T33" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U33" s="5">
         <v>2</v>
@@ -8615,7 +8616,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R34" s="5">
         <v>0</v>
@@ -8624,7 +8625,7 @@
         <v>1</v>
       </c>
       <c r="T34" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U34" s="5">
         <v>2</v>
@@ -8690,7 +8691,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R35" s="5">
         <v>0</v>
@@ -8699,7 +8700,7 @@
         <v>1</v>
       </c>
       <c r="T35" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U35" s="5">
         <v>2</v>
@@ -8765,7 +8766,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R36" s="5">
         <v>0</v>
@@ -8774,7 +8775,7 @@
         <v>3</v>
       </c>
       <c r="T36" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U36" s="5">
         <v>2</v>
@@ -8840,7 +8841,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R37" s="5">
         <v>0</v>
@@ -8849,7 +8850,7 @@
         <v>3</v>
       </c>
       <c r="T37" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U37" s="5">
         <v>2</v>
@@ -8915,7 +8916,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R38" s="5">
         <v>0</v>
@@ -8924,7 +8925,7 @@
         <v>3</v>
       </c>
       <c r="T38" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U38" s="5">
         <v>2</v>
@@ -8936,7 +8937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="15" thickBot="1">
+    <row r="39" spans="1:23" ht="15.75" thickBot="1">
       <c r="A39" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -8990,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R39" s="5">
         <v>0</v>
@@ -8999,7 +9000,7 @@
         <v>3</v>
       </c>
       <c r="T39" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U39" s="5">
         <v>2</v>
@@ -9011,7 +9012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="15" thickBot="1">
+    <row r="40" spans="1:23" ht="15.75" thickBot="1">
       <c r="A40" s="5">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -9065,7 +9066,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R40" s="5">
         <v>0</v>
@@ -9074,7 +9075,7 @@
         <v>3</v>
       </c>
       <c r="T40" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U40" s="5">
         <v>2</v>
@@ -9140,7 +9141,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R41" s="5">
         <v>0</v>
@@ -9149,7 +9150,7 @@
         <v>3</v>
       </c>
       <c r="T41" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U41" s="5">
         <v>2</v>
@@ -9161,7 +9162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="15" thickBot="1">
+    <row r="42" spans="1:23" ht="15.75" thickBot="1">
       <c r="A42" s="5">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -9215,7 +9216,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R42" s="5">
         <v>0</v>
@@ -9224,7 +9225,7 @@
         <v>3</v>
       </c>
       <c r="T42" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U42" s="5">
         <v>2</v>
@@ -9236,7 +9237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="15" thickBot="1">
+    <row r="43" spans="1:23" ht="15.75" thickBot="1">
       <c r="A43" s="5">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -9290,7 +9291,7 @@
         <v>0</v>
       </c>
       <c r="Q43" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R43" s="5">
         <v>0</v>
@@ -9299,7 +9300,7 @@
         <v>3</v>
       </c>
       <c r="T43" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U43" s="5">
         <v>2</v>
@@ -9311,7 +9312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="15" thickBot="1">
+    <row r="44" spans="1:23" ht="15.75" thickBot="1">
       <c r="A44" s="5">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -9365,17 +9366,17 @@
         <v>0</v>
       </c>
       <c r="Q44" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R44" s="5">
+        <v>0</v>
+      </c>
+      <c r="S44" s="5">
+        <v>1</v>
+      </c>
+      <c r="T44" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R44" s="5">
-        <v>0</v>
-      </c>
-      <c r="S44" s="5">
-        <v>1</v>
-      </c>
-      <c r="T44" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U44" s="5">
         <v>2</v>
       </c>
@@ -9386,7 +9387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="15" thickBot="1">
+    <row r="45" spans="1:23" ht="15.75" thickBot="1">
       <c r="A45" s="5">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -9440,17 +9441,17 @@
         <v>0</v>
       </c>
       <c r="Q45" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R45" s="5">
+        <v>0</v>
+      </c>
+      <c r="S45" s="5">
+        <v>1</v>
+      </c>
+      <c r="T45" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R45" s="5">
-        <v>0</v>
-      </c>
-      <c r="S45" s="5">
-        <v>1</v>
-      </c>
-      <c r="T45" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U45" s="5">
         <v>2</v>
       </c>
@@ -9461,7 +9462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="15" thickBot="1">
+    <row r="46" spans="1:23" ht="15.75" thickBot="1">
       <c r="A46" s="5">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -9515,17 +9516,17 @@
         <v>0</v>
       </c>
       <c r="Q46" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R46" s="5">
+        <v>0</v>
+      </c>
+      <c r="S46" s="5">
+        <v>1</v>
+      </c>
+      <c r="T46" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R46" s="5">
-        <v>0</v>
-      </c>
-      <c r="S46" s="5">
-        <v>1</v>
-      </c>
-      <c r="T46" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U46" s="5">
         <v>2</v>
       </c>
@@ -9536,7 +9537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="15" thickBot="1">
+    <row r="47" spans="1:23" ht="15.75" thickBot="1">
       <c r="A47" s="5">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -9590,7 +9591,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R47" s="5">
         <v>0</v>
@@ -9599,7 +9600,7 @@
         <v>3</v>
       </c>
       <c r="T47" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U47" s="5">
         <v>2</v>
@@ -9611,7 +9612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="15" thickBot="1">
+    <row r="48" spans="1:23" ht="15.75" thickBot="1">
       <c r="A48" s="5">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -9665,7 +9666,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R48" s="5">
         <v>0</v>
@@ -9674,7 +9675,7 @@
         <v>3</v>
       </c>
       <c r="T48" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U48" s="5">
         <v>2</v>
@@ -9686,7 +9687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="15" thickBot="1">
+    <row r="49" spans="1:23" ht="15.75" thickBot="1">
       <c r="A49" s="5">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -9740,7 +9741,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R49" s="5">
         <v>0</v>
@@ -9749,7 +9750,7 @@
         <v>4</v>
       </c>
       <c r="T49" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U49" s="5">
         <v>2</v>
@@ -9761,7 +9762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="15" thickBot="1">
+    <row r="50" spans="1:23" ht="15.75" thickBot="1">
       <c r="A50" s="5">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -9815,17 +9816,17 @@
         <v>0</v>
       </c>
       <c r="Q50" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R50" s="5">
+        <v>0</v>
+      </c>
+      <c r="S50" s="5">
+        <v>1</v>
+      </c>
+      <c r="T50" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R50" s="5">
-        <v>0</v>
-      </c>
-      <c r="S50" s="5">
-        <v>1</v>
-      </c>
-      <c r="T50" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U50" s="5">
         <v>2</v>
       </c>
@@ -9836,7 +9837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="15" thickBot="1">
+    <row r="51" spans="1:23" ht="15.75" thickBot="1">
       <c r="A51" s="5">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -9890,17 +9891,17 @@
         <v>0</v>
       </c>
       <c r="Q51" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R51" s="5">
+        <v>0</v>
+      </c>
+      <c r="S51" s="5">
+        <v>1</v>
+      </c>
+      <c r="T51" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R51" s="5">
-        <v>0</v>
-      </c>
-      <c r="S51" s="5">
-        <v>1</v>
-      </c>
-      <c r="T51" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U51" s="5">
         <v>2</v>
       </c>
@@ -9911,7 +9912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="15" thickBot="1">
+    <row r="52" spans="1:23" ht="15.75" thickBot="1">
       <c r="A52" s="5">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -9965,17 +9966,17 @@
         <v>0</v>
       </c>
       <c r="Q52" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R52" s="5">
+        <v>0</v>
+      </c>
+      <c r="S52" s="5">
+        <v>1</v>
+      </c>
+      <c r="T52" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R52" s="5">
-        <v>0</v>
-      </c>
-      <c r="S52" s="5">
-        <v>1</v>
-      </c>
-      <c r="T52" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U52" s="5">
         <v>2</v>
       </c>
@@ -9986,7 +9987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="15" thickBot="1">
+    <row r="53" spans="1:23" ht="15.75" thickBot="1">
       <c r="A53" s="5">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -10040,17 +10041,17 @@
         <v>0</v>
       </c>
       <c r="Q53" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R53" s="5">
+        <v>0</v>
+      </c>
+      <c r="S53" s="5">
+        <v>1</v>
+      </c>
+      <c r="T53" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R53" s="5">
-        <v>0</v>
-      </c>
-      <c r="S53" s="5">
-        <v>1</v>
-      </c>
-      <c r="T53" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U53" s="5">
         <v>2</v>
       </c>
@@ -10061,7 +10062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="16.2" thickBot="1">
+    <row r="54" spans="1:23" ht="15.75" thickBot="1">
       <c r="A54" s="5">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -10115,17 +10116,17 @@
         <v>0</v>
       </c>
       <c r="Q54" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R54" s="5">
+        <v>0</v>
+      </c>
+      <c r="S54" s="5">
+        <v>1</v>
+      </c>
+      <c r="T54" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R54" s="5">
-        <v>0</v>
-      </c>
-      <c r="S54" s="5">
-        <v>1</v>
-      </c>
-      <c r="T54" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U54" s="5">
         <v>2</v>
       </c>
@@ -10136,7 +10137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="16.2" thickBot="1">
+    <row r="55" spans="1:23" ht="15.75" thickBot="1">
       <c r="A55" s="5">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -10190,17 +10191,17 @@
         <v>0</v>
       </c>
       <c r="Q55" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R55" s="5">
+        <v>0</v>
+      </c>
+      <c r="S55" s="5">
+        <v>1</v>
+      </c>
+      <c r="T55" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R55" s="5">
-        <v>0</v>
-      </c>
-      <c r="S55" s="5">
-        <v>1</v>
-      </c>
-      <c r="T55" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U55" s="5">
         <v>2</v>
       </c>
@@ -10211,7 +10212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="16.2" thickBot="1">
+    <row r="56" spans="1:23" ht="15.75" thickBot="1">
       <c r="A56" s="5">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -10265,17 +10266,17 @@
         <v>0</v>
       </c>
       <c r="Q56" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R56" s="5">
+        <v>0</v>
+      </c>
+      <c r="S56" s="5">
+        <v>1</v>
+      </c>
+      <c r="T56" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R56" s="5">
-        <v>0</v>
-      </c>
-      <c r="S56" s="5">
-        <v>1</v>
-      </c>
-      <c r="T56" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U56" s="5">
         <v>2</v>
       </c>
@@ -10286,7 +10287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="16.2" thickBot="1">
+    <row r="57" spans="1:23" ht="15.75" thickBot="1">
       <c r="A57" s="5">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -10340,17 +10341,17 @@
         <v>0</v>
       </c>
       <c r="Q57" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R57" s="5">
+        <v>0</v>
+      </c>
+      <c r="S57" s="5">
+        <v>1</v>
+      </c>
+      <c r="T57" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R57" s="5">
-        <v>0</v>
-      </c>
-      <c r="S57" s="5">
-        <v>1</v>
-      </c>
-      <c r="T57" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U57" s="5">
         <v>2</v>
       </c>
@@ -10361,7 +10362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="16.2" thickBot="1">
+    <row r="58" spans="1:23" ht="15.75" thickBot="1">
       <c r="A58" s="5">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -10415,17 +10416,17 @@
         <v>0</v>
       </c>
       <c r="Q58" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R58" s="5">
+        <v>0</v>
+      </c>
+      <c r="S58" s="5">
+        <v>1</v>
+      </c>
+      <c r="T58" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R58" s="5">
-        <v>0</v>
-      </c>
-      <c r="S58" s="5">
-        <v>1</v>
-      </c>
-      <c r="T58" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U58" s="5">
         <v>2</v>
       </c>
@@ -10436,7 +10437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="16.2" thickBot="1">
+    <row r="59" spans="1:23" ht="15.75" thickBot="1">
       <c r="A59" s="5">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -10490,17 +10491,17 @@
         <v>0</v>
       </c>
       <c r="Q59" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R59" s="5">
+        <v>0</v>
+      </c>
+      <c r="S59" s="5">
+        <v>1</v>
+      </c>
+      <c r="T59" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R59" s="5">
-        <v>0</v>
-      </c>
-      <c r="S59" s="5">
-        <v>1</v>
-      </c>
-      <c r="T59" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U59" s="5">
         <v>2</v>
       </c>
@@ -10511,7 +10512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="16.2" thickBot="1">
+    <row r="60" spans="1:23" ht="15.75" thickBot="1">
       <c r="A60" s="5">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -10565,17 +10566,17 @@
         <v>0</v>
       </c>
       <c r="Q60" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R60" s="5">
+        <v>0</v>
+      </c>
+      <c r="S60" s="5">
+        <v>1</v>
+      </c>
+      <c r="T60" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R60" s="5">
-        <v>0</v>
-      </c>
-      <c r="S60" s="5">
-        <v>1</v>
-      </c>
-      <c r="T60" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U60" s="5">
         <v>2</v>
       </c>
@@ -10586,7 +10587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="16.2" thickBot="1">
+    <row r="61" spans="1:23" ht="15.75" thickBot="1">
       <c r="A61" s="5">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -10640,17 +10641,17 @@
         <v>0</v>
       </c>
       <c r="Q61" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R61" s="5">
+        <v>0</v>
+      </c>
+      <c r="S61" s="5">
+        <v>1</v>
+      </c>
+      <c r="T61" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R61" s="5">
-        <v>0</v>
-      </c>
-      <c r="S61" s="5">
-        <v>1</v>
-      </c>
-      <c r="T61" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U61" s="5">
         <v>2</v>
       </c>
@@ -10661,7 +10662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="16.2" thickBot="1">
+    <row r="62" spans="1:23" ht="15.75" thickBot="1">
       <c r="A62" s="5">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -10715,17 +10716,17 @@
         <v>0</v>
       </c>
       <c r="Q62" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R62" s="5">
+        <v>0</v>
+      </c>
+      <c r="S62" s="5">
+        <v>1</v>
+      </c>
+      <c r="T62" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R62" s="5">
-        <v>0</v>
-      </c>
-      <c r="S62" s="5">
-        <v>1</v>
-      </c>
-      <c r="T62" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U62" s="5">
         <v>2</v>
       </c>
@@ -10736,7 +10737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="16.2" thickBot="1">
+    <row r="63" spans="1:23" ht="15.75" thickBot="1">
       <c r="A63" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -10790,17 +10791,17 @@
         <v>0</v>
       </c>
       <c r="Q63" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R63" s="5">
+        <v>0</v>
+      </c>
+      <c r="S63" s="5">
+        <v>1</v>
+      </c>
+      <c r="T63" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R63" s="5">
-        <v>0</v>
-      </c>
-      <c r="S63" s="5">
-        <v>1</v>
-      </c>
-      <c r="T63" s="19" t="s">
-        <v>123</v>
-      </c>
       <c r="U63" s="5">
         <v>2</v>
       </c>
@@ -10811,7 +10812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="16.2" thickBot="1">
+    <row r="64" spans="1:23" ht="15.75" thickBot="1">
       <c r="A64" s="5">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -10865,16 +10866,16 @@
         <v>0</v>
       </c>
       <c r="Q64" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="R64" s="5">
+        <v>0</v>
+      </c>
+      <c r="S64" s="5">
+        <v>1</v>
+      </c>
+      <c r="T64" s="19" t="s">
         <v>122</v>
-      </c>
-      <c r="R64" s="5">
-        <v>0</v>
-      </c>
-      <c r="S64" s="5">
-        <v>1</v>
-      </c>
-      <c r="T64" s="19" t="s">
-        <v>123</v>
       </c>
       <c r="U64" s="5">
         <v>2</v>
@@ -10920,19 +10921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="59.5546875" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11176,18 +11177,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11232,7 +11233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.399999999999999">
+    <row r="4" spans="1:4" ht="16.5">
       <c r="A4" s="24" t="s">
         <v>16</v>
       </c>
@@ -11246,7 +11247,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999">
+    <row r="5" spans="1:4" ht="16.5">
       <c r="A5" s="23" t="s">
         <v>17</v>
       </c>
@@ -11260,7 +11261,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999">
+    <row r="6" spans="1:4" ht="16.5">
       <c r="A6" s="23" t="s">
         <v>18</v>
       </c>
@@ -11274,7 +11275,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999">
+    <row r="7" spans="1:4" ht="16.5">
       <c r="A7" s="23" t="s">
         <v>100</v>
       </c>
@@ -11290,58 +11291,58 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -11352,7 +11353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
@@ -11362,13 +11363,13 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11445,13 +11446,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999">
+    <row r="5" spans="1:6" ht="16.5">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -11465,13 +11466,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999">
+    <row r="6" spans="1:6" ht="16.5">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -11485,13 +11486,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.399999999999999">
+    <row r="7" spans="1:6" ht="16.5">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -11505,13 +11506,13 @@
         <v>3</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999">
+    <row r="8" spans="1:6" ht="16.5">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -11525,13 +11526,13 @@
         <v>4</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999">
+    <row r="9" spans="1:6" ht="16.5">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -11545,13 +11546,13 @@
         <v>5</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F9" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.399999999999999">
+    <row r="10" spans="1:6" ht="16.5">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -11565,13 +11566,13 @@
         <v>6</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.399999999999999">
+    <row r="11" spans="1:6" ht="16.5">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -11585,13 +11586,13 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.399999999999999">
+    <row r="12" spans="1:6" ht="16.5">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -11605,13 +11606,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F12" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.399999999999999">
+    <row r="13" spans="1:6" ht="16.5">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -11625,13 +11626,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.399999999999999">
+    <row r="14" spans="1:6" ht="16.5">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -11645,13 +11646,13 @@
         <v>10</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.399999999999999">
+    <row r="15" spans="1:6" ht="16.5">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -11665,13 +11666,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F15" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.399999999999999">
+    <row r="16" spans="1:6" ht="16.5">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -11685,13 +11686,13 @@
         <v>12</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F16" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.399999999999999">
+    <row r="17" spans="1:6" ht="16.5">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -11705,13 +11706,13 @@
         <v>13</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F17" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.399999999999999">
+    <row r="18" spans="1:6" ht="16.5">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -11725,13 +11726,13 @@
         <v>14</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F18" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.399999999999999">
+    <row r="19" spans="1:6" ht="16.5">
       <c r="A19" s="5">
         <v>16</v>
       </c>
@@ -11745,13 +11746,13 @@
         <v>15</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F19" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.399999999999999">
+    <row r="20" spans="1:6" ht="16.5">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -11765,13 +11766,13 @@
         <v>16</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.399999999999999">
+    <row r="21" spans="1:6" ht="16.5">
       <c r="A21" s="5">
         <v>18</v>
       </c>
@@ -11785,13 +11786,13 @@
         <v>17</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F21" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.399999999999999">
+    <row r="22" spans="1:6" ht="16.5">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -11805,13 +11806,13 @@
         <v>18</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22" s="9">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17.399999999999999">
+    <row r="23" spans="1:6" ht="16.5">
       <c r="A23" s="5">
         <v>20</v>
       </c>
@@ -11825,7 +11826,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" s="9">
         <v>120</v>
@@ -11854,17 +11855,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11872,7 +11873,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>67</v>
@@ -11881,7 +11882,7 @@
         <v>65</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>66</v>
@@ -11898,7 +11899,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>1</v>
@@ -12063,17 +12064,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>